<commit_message>
update my model summery and change weight of loc
</commit_message>
<xml_diff>
--- a/my models.xlsx
+++ b/my models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chan Kin Yan\Documents\GitHub\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B42BFA-B854-4ED4-AD0D-804958AF8680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5415FDE7-7DDF-41B6-B0C8-43785246ED56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25F5D22B-B428-4E40-8DA6-9C426A79E496}"/>
+    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{25F5D22B-B428-4E40-8DA6-9C426A79E496}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t>h5</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,213 +78,233 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>zoe_pointpillars1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoe_pointpillars2</t>
+  </si>
+  <si>
+    <t>zoe_pointpillars3</t>
+  </si>
+  <si>
+    <t>model 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wrong 32 anchors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model 9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(-50.4,23.52)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(-43.68,70.56)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(0,6.4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iou, 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max pillars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpp (iou, minpoints, diag )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iou, 1, 0.5D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kmeans 8 anchors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32 anchors correct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(-56.32, 25.6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(-46.08, 56.32)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Channels</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok/ yaw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nono</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(0, 6.4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoe_pp_yolo3</t>
+  </si>
+  <si>
+    <t>zoe_pp_yolo2</t>
+  </si>
+  <si>
+    <t>training time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30.59 mins</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>trainable params</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>epoch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upsampling, nofocus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoe_pp_yolo4</t>
+  </si>
+  <si>
+    <t>simplest no focus 3 resblock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">no focus </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(-56.32, 25.7)</t>
+  </si>
+  <si>
+    <t>(-46.08, 56.33)</t>
+  </si>
+  <si>
+    <t>(-56.32, 25.8)</t>
+  </si>
+  <si>
+    <t>(-46.08, 56.34)</t>
+  </si>
+  <si>
+    <t>zoe_pp_yolo1</t>
+  </si>
+  <si>
+    <t>(-56.32, 25.5)</t>
+  </si>
+  <si>
+    <t>(-46.08, 56.31)</t>
+  </si>
+  <si>
+    <t>(0,6.4)</t>
+  </si>
+  <si>
+    <t>4 anchors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">all </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gg think all are shit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>align iou</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoe_pp_yolo5</t>
+  </si>
+  <si>
+    <t>(-56.32, 25.9)</t>
+  </si>
+  <si>
+    <t>(-46.08, 56.35)</t>
+  </si>
+  <si>
+    <t>multi-layers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>need to redo code fkkk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>zoe_pointpillars4</t>
-  </si>
-  <si>
-    <t>zoe_pointpillars1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zoe_pointpillars2</t>
-  </si>
-  <si>
-    <t>zoe_pointpillars3</t>
-  </si>
-  <si>
-    <t>model 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>train4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wrong 32 anchors</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>train 5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>model 9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>model 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>height width ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>(-50.4,23.52)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>(-43.68,70.56)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(0,6.4)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>iou, 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max pillars</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cpp (iou, minpoints, diag )</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>iou, 1, 0.5D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kmeans 8 anchors</t>
-  </si>
-  <si>
-    <t>kmeans 8 anchors</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>32 anchors correct</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(-56.32, 25.6)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(-46.08, 56.32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Channels</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ok</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ok/ yaw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nono</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>model</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(0, 6.4)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zoe_pp_yolo3</t>
-  </si>
-  <si>
-    <t>zoe_pp_yolo2</t>
-  </si>
-  <si>
-    <t>basix</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>training time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>30.59 mins</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>trainable params</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>epoch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>upsampling, nofocus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zoe_pp_yolo4</t>
-  </si>
-  <si>
-    <t>simplest no focus 3 resblock</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">no focus </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(-56.32, 25.7)</t>
-  </si>
-  <si>
-    <t>(-46.08, 56.33)</t>
-  </si>
-  <si>
-    <t>(-56.32, 25.8)</t>
-  </si>
-  <si>
-    <t>(-46.08, 56.34)</t>
-  </si>
-  <si>
-    <t>zoe_pp_yolo1</t>
-  </si>
-  <si>
-    <t>(-56.32, 25.5)</t>
-  </si>
-  <si>
-    <t>(-46.08, 56.31)</t>
-  </si>
-  <si>
-    <t>(0,6.4)</t>
-  </si>
-  <si>
-    <t>4 anchors</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">all </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gg think all are shit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>align iou</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zoe_pp_yolo5</t>
-  </si>
-  <si>
-    <t>(-56.32, 25.9)</t>
-  </si>
-  <si>
-    <t>(-46.08, 56.35)</t>
-  </si>
-  <si>
-    <t>multi-layers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>need to redo code fkkk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>iou, 3, 0.5D</t>
+  </si>
+  <si>
+    <t>train5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -337,12 +357,36 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -359,7 +403,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -370,15 +414,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -697,13 +762,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3903BAF0-A2DE-4483-90A3-00B242B221E4}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.625" style="1" bestFit="1" customWidth="1"/>
@@ -722,62 +787,62 @@
     <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="I1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="5" t="s">
+      <c r="M1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>44</v>
+      <c r="O1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1">
         <v>4</v>
@@ -786,16 +851,16 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="J2" s="1">
         <v>8000</v>
@@ -804,13 +869,13 @@
         <v>128</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="1">
         <v>83</v>
@@ -818,10 +883,10 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1">
         <v>4</v>
@@ -830,16 +895,16 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="J3" s="1">
         <v>8000</v>
@@ -848,165 +913,212 @@
         <v>128</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3">
+    <row r="4" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="12">
         <v>2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="13">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="12">
+        <v>1000</v>
+      </c>
+      <c r="K4" s="12">
+        <v>128</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
         <v>0.16</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="3">
+      <c r="F5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="8">
         <v>1000</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K5" s="8">
         <v>128</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="4">
+      <c r="L5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" s="9">
         <v>9011272</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q5" s="8">
         <f>14</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="M5" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="1">
-        <v>8000</v>
-      </c>
-      <c r="K9" s="1">
+    <row r="9" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="11">
+        <v>1000</v>
+      </c>
+      <c r="K9" s="11">
         <v>64</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>45</v>
+      <c r="L9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="I10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J10" s="3">
         <v>1000</v>
@@ -1015,81 +1127,63 @@
         <v>64</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1000</v>
+      </c>
+      <c r="K11" s="6">
+        <v>64</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="3">
-        <v>1000</v>
-      </c>
-      <c r="K11" s="3">
-        <v>128</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="2">
-        <v>4</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="2">
-        <v>8000</v>
-      </c>
-      <c r="K15" s="2">
-        <v>64</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>